<commit_message>
hapus menu tidak terpakai
</commit_message>
<xml_diff>
--- a/htmlbox pro/leftcolumn/Fotografi videografi.xlsx
+++ b/htmlbox pro/leftcolumn/Fotografi videografi.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>Sigma</t>
+  </si>
+  <si>
+    <t>FujiFilm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic </t>
+  </si>
+  <si>
+    <t>All Brand</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +129,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,9 +151,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:F30"/>
+  <dimension ref="C1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -508,178 +524,268 @@
       </c>
     </row>
     <row r="9" spans="3:6">
-      <c r="C9">
+      <c r="C9" s="2">
+        <v>274</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="3:6">
+      <c r="C10" s="2">
+        <v>378</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="3:6">
+      <c r="C11" s="2">
+        <v>351</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="3:6">
+      <c r="C12" s="2">
+        <v>379</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="3:6">
+      <c r="C13" s="2">
+        <v>380</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="3:6">
+      <c r="C14" s="2">
+        <v>381</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="3:6">
+      <c r="C15" s="2">
+        <v>382</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="3:6">
+      <c r="C16" s="2">
+        <v>383</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="2">
+        <v>683</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18">
         <v>153</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:6">
-      <c r="C10">
+    <row r="19" spans="3:6">
+      <c r="C19">
         <v>631</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="3:6">
-      <c r="C11">
+    <row r="20" spans="3:6">
+      <c r="C20">
         <v>692</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:6">
-      <c r="C12">
+    <row r="21" spans="3:6">
+      <c r="C21">
         <v>693</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="3:6">
-      <c r="C13">
+    <row r="22" spans="3:6">
+      <c r="C22">
         <v>694</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:6">
-      <c r="C14">
+    <row r="23" spans="3:6">
+      <c r="C23">
         <v>390</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="3:6">
-      <c r="C15">
+    <row r="24" spans="3:6">
+      <c r="C24">
         <v>391</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="3:6">
-      <c r="C16">
+    <row r="25" spans="3:6">
+      <c r="C25">
         <v>393</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
-      <c r="C17">
+    <row r="26" spans="3:6">
+      <c r="C26">
         <v>708</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
-      <c r="C18">
+    <row r="27" spans="3:6">
+      <c r="C27">
         <v>709</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
-      <c r="C19">
+    <row r="28" spans="3:6">
+      <c r="C28">
         <v>396</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="3:5">
-      <c r="C20">
+    <row r="29" spans="3:6">
+      <c r="C29">
         <v>394</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E29" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
-      <c r="C21">
+    <row r="30" spans="3:6">
+      <c r="C30">
         <v>395</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
-      <c r="C22">
+    <row r="31" spans="3:6">
+      <c r="C31">
         <v>716</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
-      <c r="C23">
+    <row r="32" spans="3:6">
+      <c r="C32">
         <v>397</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="3:5">
-      <c r="C24">
+    <row r="33" spans="3:5">
+      <c r="C33">
         <v>715</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="3:5">
-      <c r="C25">
+    <row r="34" spans="3:5">
+      <c r="C34">
         <v>695</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="3:5">
-      <c r="C26">
+    <row r="35" spans="3:5">
+      <c r="C35">
         <v>723</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E35" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="3:5">
-      <c r="C27">
+    <row r="36" spans="3:5">
+      <c r="C36">
         <v>718</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E36" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
-      <c r="C28">
+    <row r="37" spans="3:5">
+      <c r="C37">
         <v>724</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
-      <c r="C29">
+    <row r="38" spans="3:5">
+      <c r="C38">
         <v>721</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E38" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
-      <c r="C30">
+    <row r="39" spans="3:5">
+      <c r="C39">
         <v>720</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E39" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>